<commit_message>
Added Physics Experiment 0314 data
</commit_message>
<xml_diff>
--- a/1st-term/Basic Physics Experiment/Assignments/2019-03-14-5조-액체의 밀도 측정-결과.xlsx
+++ b/1st-term/Basic Physics Experiment/Assignments/2019-03-14-5조-액체의 밀도 측정-결과.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bedro\Drive\2019 School\1st-term\Basic Physics Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bedro\Drive\2019 School\CAU2019\1st-term\Basic Physics Experiment\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7710" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,21 +84,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.000000000"/>
-    <numFmt numFmtId="180" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -106,7 +106,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -141,13 +141,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -209,7 +209,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -382,11 +382,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="464415688"/>
-        <c:axId val="405138248"/>
+        <c:axId val="363744160"/>
+        <c:axId val="363836496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="464415688"/>
+        <c:axId val="363744160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +445,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ko-KR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -482,10 +482,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ko-KR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405138248"/>
+        <c:crossAx val="363836496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -493,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="405138248"/>
+        <c:axId val="363836496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +565,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ko-KR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -597,10 +597,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ko-KR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464415688"/>
+        <c:crossAx val="363744160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -640,7 +640,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -670,7 +670,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ko-KR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -722,7 +722,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -841,11 +841,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="464577320"/>
-        <c:axId val="464577712"/>
+        <c:axId val="363837280"/>
+        <c:axId val="363836888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="464577320"/>
+        <c:axId val="363837280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,10 +884,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ko-KR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464577712"/>
+        <c:crossAx val="363836888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -895,7 +895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="464577712"/>
+        <c:axId val="363836888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,10 +943,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ko-KR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464577320"/>
+        <c:crossAx val="363837280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -986,7 +986,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1016,7 +1016,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ko-KR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2469,21 +2469,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="3.75" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="3.375" customWidth="1"/>
-    <col min="9" max="9" width="2.75" customWidth="1"/>
-    <col min="13" max="13" width="15.625" customWidth="1"/>
-    <col min="15" max="15" width="13.375" customWidth="1"/>
-    <col min="16" max="16" width="10.25" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -3034,21 +3034,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="3.75" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="3.375" customWidth="1"/>
-    <col min="9" max="9" width="2.75" customWidth="1"/>
-    <col min="13" max="13" width="15.625" customWidth="1"/>
-    <col min="15" max="15" width="13.375" customWidth="1"/>
-    <col min="16" max="16" width="10.25" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>